<commit_message>
This is second commit
</commit_message>
<xml_diff>
--- a/testData/input.xlsx
+++ b/testData/input.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -133,9 +133,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -591,7 +594,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>